<commit_message>
commit update 1/3/2023 23h:44'
</commit_message>
<xml_diff>
--- a/FE/Excel/OTs_Table.xlsx
+++ b/FE/Excel/OTs_Table.xlsx
@@ -14,111 +14,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <x:si>
     <x:t>id</x:t>
   </x:si>
   <x:si>
-    <x:t>type</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Date</x:t>
-  </x:si>
-  <x:si>
-    <x:t>start</x:t>
-  </x:si>
-  <x:si>
-    <x:t>end</x:t>
-  </x:si>
-  <x:si>
-    <x:t>realTime</x:t>
-  </x:si>
-  <x:si>
-    <x:t>status</x:t>
-  </x:si>
-  <x:si>
-    <x:t>description</x:t>
-  </x:si>
-  <x:si>
-    <x:t>leadCreate</x:t>
-  </x:si>
-  <x:si>
-    <x:t>dateCreate</x:t>
-  </x:si>
-  <x:si>
-    <x:t>updateUser</x:t>
-  </x:si>
-  <x:si>
-    <x:t>dateUpdate</x:t>
-  </x:si>
-  <x:si>
-    <x:t>note</x:t>
-  </x:si>
-  <x:si>
-    <x:t>user</x:t>
-  </x:si>
-  <x:si>
-    <x:t>idProject</x:t>
+    <x:t>HinhThucOT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NgayOT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NgayBatDau</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NgayKetThuc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ThoiGianThucTeOT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TrangThai</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MoTa</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TruongNhom</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NgayTao</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NguoiCapNhat</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NgayCapNhat</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LyDoHuy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NguoiOT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TenDuAn</x:t>
   </x:si>
   <x:si>
     <x:t>OT</x:t>
   </x:si>
   <x:si>
-    <x:t>18:00</x:t>
-  </x:si>
-  <x:si>
     <x:t>19:00</x:t>
   </x:si>
   <x:si>
-    <x:t>1:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>accepted</x:t>
-  </x:si>
-  <x:si>
-    <x:t>dasfdsafdasf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>leader1 vhec</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Duong Trong Nghia</x:t>
-  </x:si>
-  <x:si>
-    <x:t>thanh dien nguyen tran</x:t>
-  </x:si>
-  <x:si>
-    <x:t>IMS_Test2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>22:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>hello</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Cao Van Vinh</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nguyen Tran Thanh Dien</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Vo Vien Thien</x:t>
-  </x:si>
-  <x:si>
-    <x:t>18:30</x:t>
-  </x:si>
-  <x:si>
-    <x:t>00:30</x:t>
-  </x:si>
-  <x:si>
-    <x:t>gdfsgdfsg</x:t>
+    <x:t>19:39</x:t>
+  </x:si>
+  <x:si>
+    <x:t>00:39</x:t>
+  </x:si>
+  <x:si>
+    <x:t>process</x:t>
+  </x:si>
+  <x:si>
+    <x:t>fdsaf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Đặng Đức Long</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Võ Trung Kiên</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IMS4</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -507,27 +474,27 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:O6"/>
+  <x:dimension ref="A1:O2"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="3.420625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="5.630625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="5.030625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="12.340625" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="10.890625" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="5.800625" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="6.650625" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="9.320625" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="9.600625" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="12.530625" style="0" customWidth="1"/>
-    <x:col min="9" max="9" width="12.750625" style="0" customWidth="1"/>
-    <x:col min="10" max="10" width="16.170625" style="0" customWidth="1"/>
-    <x:col min="11" max="11" width="18.240625" style="0" customWidth="1"/>
-    <x:col min="12" max="12" width="16.170625" style="0" customWidth="1"/>
-    <x:col min="13" max="13" width="5.790625" style="0" customWidth="1"/>
-    <x:col min="14" max="14" width="22.890625" style="0" customWidth="1"/>
-    <x:col min="15" max="15" width="10.810625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="12.370625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="13.070625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="18.030625" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="10.290625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="6.760625" style="0" customWidth="1"/>
+    <x:col min="9" max="9" width="14.720625" style="0" customWidth="1"/>
+    <x:col min="10" max="10" width="14.050625" style="0" customWidth="1"/>
+    <x:col min="11" max="11" width="14.250625" style="0" customWidth="1"/>
+    <x:col min="12" max="12" width="13.510625" style="0" customWidth="1"/>
+    <x:col min="13" max="13" width="9.420625" style="0" customWidth="1"/>
+    <x:col min="14" max="14" width="13.730625" style="0" customWidth="1"/>
+    <x:col min="15" max="15" width="9.710625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:15">
@@ -579,13 +546,13 @@
     </x:row>
     <x:row r="2" spans="1:15">
       <x:c r="A2" s="1" t="n">
-        <x:v>76</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="B2" s="1" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="C2" s="2">
-        <x:v>44980</x:v>
+        <x:v>45000</x:v>
       </x:c>
       <x:c r="D2" s="1" t="s">
         <x:v>16</x:v>
@@ -606,200 +573,20 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="J2" s="3">
-        <x:v>44979.3978657292</x:v>
+        <x:v>44986.3461325</x:v>
       </x:c>
       <x:c r="K2" s="1" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="L2" s="3">
-        <x:v>44979.4093468056</x:v>
+        <x:v>44986.3461325</x:v>
       </x:c>
       <x:c r="M2" s="1" t="s"/>
       <x:c r="N2" s="1" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="O2" s="1" t="s">
         <x:v>23</x:v>
-      </x:c>
-      <x:c r="O2" s="1" t="s">
-        <x:v>24</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:15">
-      <x:c r="A3" s="1" t="n">
-        <x:v>86</x:v>
-      </x:c>
-      <x:c r="B3" s="1" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C3" s="2">
-        <x:v>44980</x:v>
-      </x:c>
-      <x:c r="D3" s="1" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="E3" s="1" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="F3" s="1" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="G3" s="1" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="H3" s="1" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="I3" s="1" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="J3" s="3">
-        <x:v>44979.4313254977</x:v>
-      </x:c>
-      <x:c r="K3" s="1" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="L3" s="3">
-        <x:v>44979.4337807176</x:v>
-      </x:c>
-      <x:c r="M3" s="1" t="s"/>
-      <x:c r="N3" s="1" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="O3" s="1" t="s">
-        <x:v>24</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:15">
-      <x:c r="A4" s="1" t="n">
-        <x:v>87</x:v>
-      </x:c>
-      <x:c r="B4" s="1" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C4" s="2">
-        <x:v>44980</x:v>
-      </x:c>
-      <x:c r="D4" s="1" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="E4" s="1" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="F4" s="1" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="G4" s="1" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="H4" s="1" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="I4" s="1" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="J4" s="3">
-        <x:v>44979.4313254977</x:v>
-      </x:c>
-      <x:c r="K4" s="1" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="L4" s="3">
-        <x:v>44979.4340037037</x:v>
-      </x:c>
-      <x:c r="M4" s="1" t="s"/>
-      <x:c r="N4" s="1" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="O4" s="1" t="s">
-        <x:v>24</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:15">
-      <x:c r="A5" s="1" t="n">
-        <x:v>78</x:v>
-      </x:c>
-      <x:c r="B5" s="1" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C5" s="2">
-        <x:v>44980</x:v>
-      </x:c>
-      <x:c r="D5" s="1" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="E5" s="1" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="F5" s="1" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="G5" s="1" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="H5" s="1" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="I5" s="1" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="J5" s="3">
-        <x:v>44979.3978657292</x:v>
-      </x:c>
-      <x:c r="K5" s="1" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="L5" s="3">
-        <x:v>44979.4069594444</x:v>
-      </x:c>
-      <x:c r="M5" s="1" t="s"/>
-      <x:c r="N5" s="1" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="O5" s="1" t="s">
-        <x:v>24</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:15">
-      <x:c r="A6" s="1" t="n">
-        <x:v>82</x:v>
-      </x:c>
-      <x:c r="B6" s="1" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C6" s="2">
-        <x:v>44980</x:v>
-      </x:c>
-      <x:c r="D6" s="1" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="E6" s="1" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="F6" s="1" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="G6" s="1" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="H6" s="1" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="I6" s="1" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="J6" s="3">
-        <x:v>44979.4309327199</x:v>
-      </x:c>
-      <x:c r="K6" s="1" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="L6" s="3">
-        <x:v>44979.4318824537</x:v>
-      </x:c>
-      <x:c r="M6" s="1" t="s"/>
-      <x:c r="N6" s="1" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="O6" s="1" t="s">
-        <x:v>24</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>